<commit_message>
Update Excel files from OneDrive - Sat Jun 28 12:59:03 UTC 2025
</commit_message>
<xml_diff>
--- a/data/RND_Todos.xlsx
+++ b/data/RND_Todos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29022"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28486927-638A-4BDD-A540-B5A0917C9B6B}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{252D3C94-FA86-4E30-9158-F87BF8333896}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,21 @@
     <t>CREATED_DATE</t>
   </si>
   <si>
+    <t>Sample witnessing and submission to be done to PVEL for retesting</t>
+  </si>
+  <si>
+    <t>GK</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
     <t>TODO_ID</t>
   </si>
   <si>
@@ -69,6 +84,9 @@
   </si>
   <si>
     <t>MEETING_DATE</t>
+  </si>
+  <si>
+    <t>after receiving new component we will submit the sample in july</t>
   </si>
   <si>
     <t>ATTENDEES</t>
@@ -87,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +119,17 @@
       <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Aptos Display"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,13 +147,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,6 +549,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" ht="115.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -506,10 +576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8167951-320E-48E2-BC08-F697F42D5DFF}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,19 +589,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="130.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +622,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -556,21 +634,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Sat Jun 28 13:22:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/RND_Todos.xlsx
+++ b/data/RND_Todos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29022"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{252D3C94-FA86-4E30-9158-F87BF8333896}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8984E873-9477-4153-BAC7-3D2CA4E5F16B}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,6 +175,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +513,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,6 +569,12 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="4">
+        <v>45838</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45805</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -579,7 +586,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,6 +614,9 @@
     <row r="2" spans="1:5" ht="130.5">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>45835</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>

</xml_diff>